<commit_message>
added storypoints and inserted canvas for scene3
</commit_message>
<xml_diff>
--- a/ProjectManagment.xlsx
+++ b/ProjectManagment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Schule\AEC\AECProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Schule\4AHIF\SYP\DeepSpaceProject - Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE99AE04-DCF5-4620-8A88-6409EE4AF297}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A084525-AC65-4220-90C0-B26BAE22839E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3840" yWindow="2745" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="82">
   <si>
     <t>Initial</t>
   </si>
@@ -256,6 +256,30 @@
   </si>
   <si>
     <t>Story-12</t>
+  </si>
+  <si>
+    <t>Scene3 - Create Canvas on the floor</t>
+  </si>
+  <si>
+    <t>Scene3 - Create different packet prefabs</t>
+  </si>
+  <si>
+    <t>Scene3 - Create 3 slot objects and slot absorbs packets it gets in touch with</t>
+  </si>
+  <si>
+    <t>Scene3 - Packet sticks to Person if the person gets in touch with packet</t>
+  </si>
+  <si>
+    <t>Scene3 - Create Packet Factory</t>
+  </si>
+  <si>
+    <t>Scene3 - Create object, that measures the time of the game</t>
+  </si>
+  <si>
+    <t>Scene3 - Save score to file</t>
+  </si>
+  <si>
+    <t>13 SP sind aufgeteilt worden</t>
   </si>
 </sst>
 </file>
@@ -267,7 +291,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,6 +332,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -405,7 +436,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
@@ -483,13 +514,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1217,12 +1254,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="A1" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1254,19 +1291,19 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
     </row>
     <row r="6" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -2041,7 +2078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
@@ -2528,7 +2565,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="29">
+      <c r="A33" s="27">
         <v>43959</v>
       </c>
     </row>
@@ -2613,7 +2650,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="29">
+      <c r="A39" s="27">
         <v>43962</v>
       </c>
     </row>
@@ -2666,10 +2703,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2871,11 +2908,11 @@
       <c r="A13" s="16">
         <v>12</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="17">
-        <v>13</v>
+      <c r="C13" s="31" t="s">
+        <v>81</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
@@ -2974,7 +3011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="24">
         <v>20</v>
       </c>
@@ -2995,6 +3032,9 @@
       <c r="C22" s="26">
         <v>1</v>
       </c>
+      <c r="E22" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="24">
@@ -3005,6 +3045,86 @@
       </c>
       <c r="C23" s="26">
         <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="26">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="39" x14ac:dyDescent="0.25">
+      <c r="A25" s="24">
+        <v>24</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="24">
+        <v>25</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="24">
+        <v>26</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="24">
+        <v>27</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="39" x14ac:dyDescent="0.25">
+      <c r="A29" s="24">
+        <v>28</v>
+      </c>
+      <c r="B29" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="24">
+        <v>29</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="26">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
latest status from 18-05-20
</commit_message>
<xml_diff>
--- a/ProjectManagment.xlsx
+++ b/ProjectManagment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Schule\AEC\AECProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Schule\4AHIF\SYP\DeepSpaceProject - Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30ACB4B-C73B-47ED-ADE2-17548D90195A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2559CC24-DB8B-4A60-BC5C-E9F25B96DB25}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="89">
   <si>
     <t>Initial</t>
   </si>
@@ -295,6 +295,12 @@
   </si>
   <si>
     <t>Story-24</t>
+  </si>
+  <si>
+    <t>Adapt to double instance</t>
+  </si>
+  <si>
+    <t>Animation scene2 encryption</t>
   </si>
 </sst>
 </file>
@@ -536,14 +542,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -611,10 +617,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Burndown!$A$7:$A$52</c:f>
+              <c:f>Burndown!$A$7:$A$56</c:f>
               <c:numCache>
                 <c:formatCode>mmm\ d", "yyyy</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
                   <c:v>43857</c:v>
                 </c:pt>
@@ -671,16 +677,28 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>44109</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44123</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44137</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44151</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44165</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Burndown!$J$7:$J$52</c:f>
+              <c:f>Burndown!$J$7:$J$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="50"/>
                 <c:pt idx="0" formatCode="0.0">
                   <c:v>39</c:v>
                 </c:pt>
@@ -706,36 +724,48 @@
                   <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>26.720588235294116</c:v>
+                  <c:v>29.720588235294116</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>19.441176470588232</c:v>
+                  <c:v>22.441176470588232</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12.16176470588235</c:v>
+                  <c:v>15.16176470588235</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.8823529411764675</c:v>
+                  <c:v>20.882352941176464</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>20.882352941176464</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20.882352941176464</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20.882352941176464</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20.882352941176464</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17.242647058823522</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.9632352941176396</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.6838235294117574</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="20">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="21">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1260,10 +1290,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,12 +1302,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
+      <c r="A1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1309,19 +1339,19 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
     </row>
     <row r="6" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -1376,7 +1406,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="7">
-        <f t="shared" ref="H7:H25" si="0">G7+D7</f>
+        <f t="shared" ref="H7:H29" si="0">G7+D7</f>
         <v>0</v>
       </c>
       <c r="I7" s="7">
@@ -1420,7 +1450,7 @@
         <v>10</v>
       </c>
       <c r="I8" s="7">
-        <f t="shared" ref="I8:I25" si="1">I7+E7</f>
+        <f t="shared" ref="I8:I24" si="1">I7+E7</f>
         <v>0</v>
       </c>
       <c r="J8" s="7">
@@ -1434,7 +1464,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <f t="shared" ref="A9:A25" si="2">A8+14</f>
+        <f t="shared" ref="A9:A29" si="2">A8+14</f>
         <v>43885</v>
       </c>
       <c r="B9" s="6">
@@ -1444,11 +1474,11 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="7">
-        <f t="shared" ref="F9:F25" si="3">J8+C9</f>
+        <f t="shared" ref="F9:F24" si="3">J8+C9</f>
         <v>29</v>
       </c>
       <c r="G9" s="7">
-        <f t="shared" ref="G9:G25" si="4">H8</f>
+        <f t="shared" ref="G9:G24" si="4">H8</f>
         <v>10</v>
       </c>
       <c r="H9" s="7">
@@ -1542,11 +1572,11 @@
         <v>70</v>
       </c>
       <c r="J11" s="7">
-        <f t="shared" ref="J11:J25" si="5">MAX(IF(OR(ISBLANK(D11),ISBLANK(E11)),F11-K10*B11,F11-D11),0)</f>
+        <f t="shared" ref="J11:J24" si="5">MAX(IF(OR(ISBLANK(D11),ISBLANK(E11)),F11-K10*B11,F11-D11),0)</f>
         <v>17</v>
       </c>
       <c r="K11" s="9">
-        <f t="shared" ref="K11:K25" si="6">IF(OR(ISBLANK(D11),ISBLANK(E11)),K10,H11/(I11+E11))</f>
+        <f t="shared" ref="K11:K24" si="6">IF(OR(ISBLANK(D11),ISBLANK(E11)),K10,H11/(I11+E11))</f>
         <v>0.2</v>
       </c>
     </row>
@@ -1678,12 +1708,14 @@
       <c r="B15" s="6">
         <v>30</v>
       </c>
-      <c r="C15" s="6"/>
+      <c r="C15" s="6">
+        <v>3</v>
+      </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="7">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G15" s="7">
         <f t="shared" si="4"/>
@@ -1699,7 +1731,7 @@
       </c>
       <c r="J15" s="7">
         <f t="shared" si="5"/>
-        <v>26.720588235294116</v>
+        <v>29.720588235294116</v>
       </c>
       <c r="K15" s="9">
         <f t="shared" si="6"/>
@@ -1719,7 +1751,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="7">
         <f t="shared" si="3"/>
-        <v>26.720588235294116</v>
+        <v>29.720588235294116</v>
       </c>
       <c r="G16" s="7">
         <f t="shared" si="4"/>
@@ -1735,7 +1767,7 @@
       </c>
       <c r="J16" s="7">
         <f t="shared" si="5"/>
-        <v>19.441176470588232</v>
+        <v>22.441176470588232</v>
       </c>
       <c r="K16" s="9">
         <f t="shared" si="6"/>
@@ -1755,7 +1787,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="7">
         <f t="shared" si="3"/>
-        <v>19.441176470588232</v>
+        <v>22.441176470588232</v>
       </c>
       <c r="G17" s="7">
         <f t="shared" si="4"/>
@@ -1771,7 +1803,7 @@
       </c>
       <c r="J17" s="7">
         <f t="shared" si="5"/>
-        <v>12.16176470588235</v>
+        <v>15.16176470588235</v>
       </c>
       <c r="K17" s="9">
         <f t="shared" si="6"/>
@@ -1786,12 +1818,14 @@
       <c r="B18" s="6">
         <v>30</v>
       </c>
-      <c r="C18" s="6"/>
+      <c r="C18" s="6">
+        <v>13</v>
+      </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="7">
         <f t="shared" si="3"/>
-        <v>12.16176470588235</v>
+        <v>28.161764705882348</v>
       </c>
       <c r="G18" s="7">
         <f t="shared" si="4"/>
@@ -1807,7 +1841,7 @@
       </c>
       <c r="J18" s="7">
         <f t="shared" si="5"/>
-        <v>4.8823529411764675</v>
+        <v>20.882352941176464</v>
       </c>
       <c r="K18" s="9">
         <f t="shared" si="6"/>
@@ -1820,14 +1854,14 @@
         <v>44025</v>
       </c>
       <c r="B19" s="6">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="7">
         <f t="shared" si="3"/>
-        <v>4.8823529411764675</v>
+        <v>20.882352941176464</v>
       </c>
       <c r="G19" s="7">
         <f t="shared" si="4"/>
@@ -1843,7 +1877,7 @@
       </c>
       <c r="J19" s="7">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>20.882352941176464</v>
       </c>
       <c r="K19" s="9">
         <f t="shared" si="6"/>
@@ -1856,14 +1890,14 @@
         <v>44039</v>
       </c>
       <c r="B20" s="6">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>20.882352941176464</v>
       </c>
       <c r="G20" s="7">
         <f t="shared" si="4"/>
@@ -1879,7 +1913,7 @@
       </c>
       <c r="J20" s="7">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>20.882352941176464</v>
       </c>
       <c r="K20" s="9">
         <f t="shared" si="6"/>
@@ -1892,14 +1926,14 @@
         <v>44053</v>
       </c>
       <c r="B21" s="6">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>20.882352941176464</v>
       </c>
       <c r="G21" s="7">
         <f t="shared" si="4"/>
@@ -1915,7 +1949,7 @@
       </c>
       <c r="J21" s="7">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>20.882352941176464</v>
       </c>
       <c r="K21" s="9">
         <f t="shared" si="6"/>
@@ -1928,14 +1962,14 @@
         <v>44067</v>
       </c>
       <c r="B22" s="6">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>20.882352941176464</v>
       </c>
       <c r="G22" s="7">
         <f t="shared" si="4"/>
@@ -1951,7 +1985,7 @@
       </c>
       <c r="J22" s="7">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>20.882352941176464</v>
       </c>
       <c r="K22" s="9">
         <f t="shared" si="6"/>
@@ -1964,14 +1998,14 @@
         <v>44081</v>
       </c>
       <c r="B23" s="6">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>20.882352941176464</v>
       </c>
       <c r="G23" s="7">
         <f t="shared" si="4"/>
@@ -1987,7 +2021,7 @@
       </c>
       <c r="J23" s="7">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>17.242647058823522</v>
       </c>
       <c r="K23" s="9">
         <f t="shared" si="6"/>
@@ -2007,7 +2041,7 @@
       <c r="E24" s="6"/>
       <c r="F24" s="7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>17.242647058823522</v>
       </c>
       <c r="G24" s="7">
         <f t="shared" si="4"/>
@@ -2023,7 +2057,7 @@
       </c>
       <c r="J24" s="7">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>9.9632352941176396</v>
       </c>
       <c r="K24" s="9">
         <f t="shared" si="6"/>
@@ -2032,7 +2066,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <f t="shared" si="2"/>
+        <f>A24+14</f>
         <v>44109</v>
       </c>
       <c r="B25" s="6">
@@ -2042,11 +2076,11 @@
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>J24+C25</f>
+        <v>9.9632352941176396</v>
       </c>
       <c r="G25" s="7">
-        <f t="shared" si="4"/>
+        <f>H24</f>
         <v>33</v>
       </c>
       <c r="H25" s="7">
@@ -2054,39 +2088,183 @@
         <v>33</v>
       </c>
       <c r="I25" s="7">
-        <f t="shared" si="1"/>
+        <f>I24+E24</f>
         <v>136</v>
       </c>
       <c r="J25" s="7">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f>MAX(IF(OR(ISBLANK(D25),ISBLANK(E25)),F25-K24*B25,F25-D25),0)</f>
+        <v>2.6838235294117574</v>
       </c>
       <c r="K25" s="9">
-        <f t="shared" si="6"/>
+        <f>IF(OR(ISBLANK(D25),ISBLANK(E25)),K24,H25/(I25+E25))</f>
         <v>0.24264705882352941</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="11">
-        <f ca="1">SUM(B7:B31)</f>
+      <c r="A26" s="5">
+        <f t="shared" si="2"/>
+        <v>44123</v>
+      </c>
+      <c r="B26" s="6">
+        <v>30</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="7">
+        <f t="shared" ref="F26:F29" si="7">J25+C26</f>
+        <v>2.6838235294117574</v>
+      </c>
+      <c r="G26" s="7">
+        <f t="shared" ref="G26:G29" si="8">H25</f>
+        <v>33</v>
+      </c>
+      <c r="H26" s="7">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="I26" s="7">
+        <f t="shared" ref="I26:I29" si="9">I25+E25</f>
+        <v>136</v>
+      </c>
+      <c r="J26" s="7">
+        <f t="shared" ref="J26:J29" si="10">MAX(IF(OR(ISBLANK(D26),ISBLANK(E26)),F26-K25*B26,F26-D26),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K26" s="9">
+        <f t="shared" ref="K26:K29" si="11">IF(OR(ISBLANK(D26),ISBLANK(E26)),K25,H26/(I26+E26))</f>
+        <v>0.24264705882352941</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <f t="shared" si="2"/>
+        <v>44137</v>
+      </c>
+      <c r="B27" s="6">
+        <v>30</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="7">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="7">
+        <f t="shared" si="8"/>
+        <v>33</v>
+      </c>
+      <c r="H27" s="7">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="I27" s="7">
+        <f t="shared" si="9"/>
+        <v>136</v>
+      </c>
+      <c r="J27" s="7">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="9">
+        <f t="shared" si="11"/>
+        <v>0.24264705882352941</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <f t="shared" si="2"/>
+        <v>44151</v>
+      </c>
+      <c r="B28" s="6">
+        <v>30</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="7">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G28" s="7">
+        <f t="shared" si="8"/>
+        <v>33</v>
+      </c>
+      <c r="H28" s="7">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="I28" s="7">
+        <f t="shared" si="9"/>
+        <v>136</v>
+      </c>
+      <c r="J28" s="7">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K28" s="9">
+        <f t="shared" si="11"/>
+        <v>0.24264705882352941</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <f t="shared" si="2"/>
+        <v>44165</v>
+      </c>
+      <c r="B29" s="6">
+        <v>30</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="7">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G29" s="7">
+        <f t="shared" si="8"/>
+        <v>33</v>
+      </c>
+      <c r="H29" s="7">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="I29" s="7">
+        <f t="shared" si="9"/>
+        <v>136</v>
+      </c>
+      <c r="J29" s="7">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K29" s="9">
+        <f t="shared" si="11"/>
+        <v>0.24264705882352941</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="10"/>
+      <c r="B30" s="11">
+        <f ca="1">SUM(B7:B35)</f>
         <v>230</v>
       </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11">
-        <f ca="1">AVERAGE(D7:D52)</f>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11">
+        <f ca="1">AVERAGE(D7:D56)</f>
         <v>4</v>
       </c>
-      <c r="E26" s="11">
-        <f ca="1">AVERAGE(E7:E52)</f>
+      <c r="E30" s="11">
+        <f ca="1">AVERAGE(E7:E56)</f>
         <v>19.166666666666668</v>
       </c>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="12"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2102,7 +2280,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
@@ -2875,10 +3053,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2889,7 +3067,7 @@
     <col min="6" max="6" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>38</v>
       </c>
@@ -2902,7 +3080,7 @@
       <c r="D1" s="15"/>
       <c r="E1" s="15"/>
     </row>
-    <row r="2" spans="1:7" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16">
         <v>1</v>
       </c>
@@ -2917,7 +3095,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16">
         <v>2</v>
       </c>
@@ -2931,11 +3109,8 @@
       <c r="E3" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="G3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:6" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16">
         <v>3</v>
       </c>
@@ -2950,7 +3125,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16">
         <v>4</v>
       </c>
@@ -2965,7 +3140,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16">
         <v>5</v>
       </c>
@@ -2983,7 +3158,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16">
         <v>6</v>
       </c>
@@ -3001,7 +3176,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16">
         <v>7</v>
       </c>
@@ -3016,7 +3191,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16">
         <v>8</v>
       </c>
@@ -3031,7 +3206,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16">
         <v>9</v>
       </c>
@@ -3049,7 +3224,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16">
         <v>10</v>
       </c>
@@ -3065,7 +3240,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16">
         <v>11</v>
       </c>
@@ -3081,7 +3256,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16">
         <v>12</v>
       </c>
@@ -3094,7 +3269,7 @@
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
     </row>
-    <row r="14" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16">
         <v>13</v>
       </c>
@@ -3107,7 +3282,7 @@
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
     </row>
-    <row r="15" spans="1:7" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16">
         <v>14</v>
       </c>
@@ -3120,7 +3295,7 @@
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
     </row>
-    <row r="16" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="21">
         <v>15</v>
       </c>
@@ -3176,7 +3351,7 @@
       <c r="C19" s="26">
         <v>1</v>
       </c>
-      <c r="E19" s="32" t="s">
+      <c r="E19" s="30" t="s">
         <v>42</v>
       </c>
       <c r="F19" s="19" t="s">
@@ -3317,6 +3492,28 @@
       </c>
       <c r="C30" s="26">
         <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="24">
+        <v>30</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="26">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="24">
+        <v>31</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" s="26">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created packet prefabs and those stick to TrackingEntities, if they get to touch each other
</commit_message>
<xml_diff>
--- a/ProjectManagment.xlsx
+++ b/ProjectManagment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Schule\4AHIF\SYP\DeepSpaceProject - Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2559CC24-DB8B-4A60-BC5C-E9F25B96DB25}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE34C84E-C0C3-4418-9490-34DB11489C5D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3840" yWindow="2745" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="89">
   <si>
     <t>Initial</t>
   </si>
@@ -3055,8 +3055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3295,7 +3295,7 @@
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
     </row>
-    <row r="16" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="21">
         <v>15</v>
       </c>
@@ -3310,7 +3310,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A17" s="24">
         <v>16</v>
       </c>
@@ -3438,6 +3438,9 @@
       <c r="C25" s="26">
         <v>2</v>
       </c>
+      <c r="E25" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="26" spans="1:6" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A26" s="24">
@@ -3459,6 +3462,9 @@
       </c>
       <c r="C27" s="26">
         <v>2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">

</xml_diff>